<commit_message>
change of test cases and adding of waitmethods and some configurations
</commit_message>
<xml_diff>
--- a/dataSource/testData.xlsx
+++ b/dataSource/testData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29452C3C-A8A3-46D1-B78C-51EA47895587}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2610" yWindow="520" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>url</t>
   </si>
@@ -65,19 +66,64 @@
     <t>1920,980</t>
   </si>
   <si>
-    <t>1900,970</t>
-  </si>
-  <si>
-    <t>1900,950</t>
-  </si>
-  <si>
     <t>https://www.unitymedia.de/privatkunden/showcase-komponenten/jan-test/aufnahmefunktion</t>
+  </si>
+  <si>
+    <t>548,602</t>
+  </si>
+  <si>
+    <t>https://www.unitymedia.de/</t>
+  </si>
+  <si>
+    <t>UM Homepage</t>
+  </si>
+  <si>
+    <t>1000,300</t>
+  </si>
+  <si>
+    <t>1220,520</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>https://www.unitymedia.de/privatkunden/logout/</t>
+  </si>
+  <si>
+    <t>https://www.unitymedia.de/privatkunden/hilfe_service/hilfe_themen/</t>
+  </si>
+  <si>
+    <t>Hilfe-Service-Übersicht</t>
+  </si>
+  <si>
+    <t>https://www.unitymedia.de/privatkunden/telefon/festnetz-optionen/komfort-option/</t>
+  </si>
+  <si>
+    <t>KOMFORT-Option</t>
+  </si>
+  <si>
+    <t>https://www.unitymedia.de/privatkunden/angebote/aktionen/meine-angebote/</t>
+  </si>
+  <si>
+    <t>Meine Angebote</t>
+  </si>
+  <si>
+    <t>UM Homepage IE</t>
+  </si>
+  <si>
+    <t>940,819</t>
+  </si>
+  <si>
+    <t>1920,945</t>
+  </si>
+  <si>
+    <t>810,600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,11 +176,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -408,29 +455,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="51.5703125" customWidth="1"/>
+    <col min="2" max="2" width="81.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" customWidth="1"/>
+    <col min="4" max="4" width="51.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -444,31 +491,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -476,22 +523,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B3"/>
+    <sheetView topLeftCell="B1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="76.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -505,109 +552,165 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.unitymedia.de/privatkunden/hilfe_service/horizon-tv/aufnahmefunktion.html"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3EA5DE85-F073-4D4F-A2F6-B92933E967B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="76.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://www.unitymedia.de/privatkunden/hilfe_service/horizon-tv/aufnahmefunktion.html" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{CB7AAB8E-E98A-42C2-A807-BF5494AEE826}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{F96BDC11-02B9-4426-B35D-8B2A6C6CA074}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{5E1F9F8F-5BBB-4888-8BF5-51D7DA8C629C}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{2AAA273E-C5C8-4C1E-92FB-32EFABC6C5EB}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{3136602C-8829-429F-98A5-B4B6D30ED9B4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="76.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -621,9 +724,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -632,34 +735,40 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.unitymedia.de/privatkunden/hilfe_service/horizon-tv/aufnahmefunktion.html"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.unitymedia.de/privatkunden/hilfe_service/horizon-tv/aufnahmefunktion.html" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{79AFEE79-A5E8-4FBF-B5F1-55E5702DEE85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -667,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -677,26 +786,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="76.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -710,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -726,8 +836,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>